<commit_message>
Changes to notebook 11; See issues #48 and #49
</commit_message>
<xml_diff>
--- a/notebooks/Data/data.xlsx
+++ b/notebooks/Data/data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/verhaarpaf/Documents/AdvancedPythonCourse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/verhaarpaf/Documents/PythonCourse/python-tutorial/notebooks/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B809F2FA-E6F6-1145-9904-71CCE1C84F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457F9E26-1E8E-2F4B-9F6C-4E98C217556C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15800" xr2:uid="{71B5851B-D6D4-6640-A230-99AA628BE8B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>A</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>7.0</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -116,9 +119,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,7 +141,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -425,7 +429,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -433,15 +437,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F9383F-031E-3642-B697-157453F356EE}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F10:F16"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,8 +461,11 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>12</v>
       </c>
@@ -474,8 +481,11 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="F2" s="2">
+        <v>44682</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>14</v>
       </c>
@@ -491,8 +501,11 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <v>44713</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>15</v>
       </c>
@@ -508,8 +521,11 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="F4" s="2">
+        <v>44743</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>8</v>
       </c>
@@ -525,8 +541,11 @@
       <c r="E5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="F5" s="2">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>10</v>
       </c>
@@ -542,8 +561,11 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="F6" s="2">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -559,17 +581,20 @@
       <c r="E7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="F7" s="2">
+        <v>44835</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="3:3" ht="17" x14ac:dyDescent="0.25">

</xml_diff>